<commit_message>
All updated for 30 industry and 40 product IE.Not tested yet.
</commit_message>
<xml_diff>
--- a/ConcordanceLibrary/LabelsAndCodes/Ind20Pro22v1_BaseSectorClassification.xlsx
+++ b/ConcordanceLibrary/LabelsAndCodes/Ind20Pro22v1_BaseSectorClassification.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\ConcordanceLibrary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\ConcordanceLibrary\LabelsAndCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="717"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="717" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BaseIndustries" sheetId="8" r:id="rId1"/>
-    <sheet name="BaseProducts" sheetId="7" r:id="rId2"/>
+    <sheet name="BaseProcesses" sheetId="8" r:id="rId1"/>
+    <sheet name="BaseFlows" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Flat rolled products</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>Liquid steel (EAF)</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Recycling</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -495,7 +513,7 @@
   </sheetPr>
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
@@ -682,10 +700,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,188 +711,257 @@
     <col min="1" max="1" width="5.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>